<commit_message>
Commit automático via script Python
</commit_message>
<xml_diff>
--- a/data (2).xlsx
+++ b/data (2).xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Export" sheetId="1" r:id="R724a495bbd0345ef"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Export" sheetId="1" r:id="R127914a29baf4769"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -31097,62 +31097,6 @@
       </x:c>
       <x:c t="inlineStr">
         <x:is>
-          <x:t>GO338044453</x:t>
-        </x:is>
-      </x:c>
-      <x:c t="inlineStr">
-        <x:is>
-          <x:t>ANTONIO WANDERSON DA CONCEIÇÃO</x:t>
-        </x:is>
-      </x:c>
-      <x:c s="8">
-        <x:v>44816</x:v>
-      </x:c>
-      <x:c t="inlineStr">
-        <x:is>
-          <x:t>MASTERCARD</x:t>
-        </x:is>
-      </x:c>
-      <x:c t="inlineStr">
-        <x:is>
-          <x:t>62994324228</x:t>
-        </x:is>
-      </x:c>
-      <x:c t="inlineStr">
-        <x:is>
-          <x:t>PLINKIN1936@GMAIL.COM</x:t>
-        </x:is>
-      </x:c>
-      <x:c t="inlineStr">
-        <x:is>
-          <x:t>CARINA SALES AGOSTINHO</x:t>
-        </x:is>
-      </x:c>
-      <x:c s="9">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c s="9">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c t="inlineStr">
-        <x:is>
-          <x:t>CEP 74425098</x:t>
-        </x:is>
-      </x:c>
-    </x:row>
-    <x:row>
-      <x:c t="inlineStr">
-        <x:is>
-          <x:t>CENTRO OESTE</x:t>
-        </x:is>
-      </x:c>
-      <x:c t="inlineStr">
-        <x:is>
-          <x:t>GOIANIA CENTRO NORTE</x:t>
-        </x:is>
-      </x:c>
-      <x:c t="inlineStr">
-        <x:is>
           <x:t>GO338050785</x:t>
         </x:is>
       </x:c>

</xml_diff>